<commit_message>
[ADD] New normalize way
</commit_message>
<xml_diff>
--- a/data/Prioridades/PC_Crimenes_Norm.xlsx
+++ b/data/Prioridades/PC_Crimenes_Norm.xlsx
@@ -95,11 +95,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -346,7 +344,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>0.0257</v>
+        <v>0.010462377812505126</v>
       </c>
       <c r="C3" s="2">
         <v>0.277</v>
@@ -357,7 +355,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>0.05294200000000001</v>
+        <v>0.02155249829376056</v>
       </c>
       <c r="C4" s="2">
         <v>0.132</v>
@@ -368,7 +366,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0.10588400000000002</v>
+        <v>0.04310499658752112</v>
       </c>
       <c r="C5" s="2">
         <v>0.086</v>
@@ -379,7 +377,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>0.1285</v>
+        <v>0.05231188906252563</v>
       </c>
       <c r="C6" s="2">
         <v>0.058</v>
@@ -390,7 +388,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>0.158826</v>
+        <v>0.06465749488128168</v>
       </c>
       <c r="C7" s="2">
         <v>0.032</v>
@@ -401,7 +399,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3">
-        <v>0.2056</v>
+        <v>0.083699022500041</v>
       </c>
       <c r="C8" s="2">
         <v>0.029</v>
@@ -412,7 +410,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>0.21176800000000004</v>
+        <v>0.08620999317504224</v>
       </c>
       <c r="C9" s="2">
         <v>0.026</v>
@@ -423,7 +421,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3">
-        <v>0.26471</v>
+        <v>0.1077624914688028</v>
       </c>
       <c r="C10" s="2">
         <v>0.023</v>

</xml_diff>